<commit_message>
第十三次提交： 测试报告的生成 引入 HTMLTestReportCN.py runner包 -- run_all_cases.py
测试报告中增加截图
base_page.py
selenium_base_case.py TearDown
</commit_message>
<xml_diff>
--- a/test_datas/test_data_infos.xlsx
+++ b/test_datas/test_data_infos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31">
   <si>
     <t>测试方法名称</t>
   </si>
@@ -87,25 +87,28 @@
     <t>是</t>
   </si>
   <si>
+    <t>测试人员</t>
+  </si>
+  <si>
+    <t>username=test01</t>
+  </si>
+  <si>
+    <t>password=newdream123</t>
+  </si>
+  <si>
+    <t>test_login_fail</t>
+  </si>
+  <si>
+    <t>验证错误的用户名和密码能否成功处理</t>
+  </si>
+  <si>
+    <t>登录失败，请检查您的用户名或密码是否填写正确。</t>
+  </si>
+  <si>
+    <t>password=newdream</t>
+  </si>
+  <si>
     <t>测试人员1</t>
-  </si>
-  <si>
-    <t>username=test01</t>
-  </si>
-  <si>
-    <t>password=newdream123</t>
-  </si>
-  <si>
-    <t>test_login_fail</t>
-  </si>
-  <si>
-    <t>验证错误的用户名和密码能否成功处理</t>
-  </si>
-  <si>
-    <t>登录失败，请检查您的用户名或密码是否填写正确。</t>
-  </si>
-  <si>
-    <t>password=newdream</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1074,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="2"/>
@@ -1266,7 +1269,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>24</v>
@@ -1375,7 +1378,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>24</v>

</xml_diff>